<commit_message>
add simulation using real genotypes
</commit_message>
<xml_diff>
--- a/Figure_data/figure6.xlsx
+++ b/Figure_data/figure6.xlsx
@@ -496,7 +496,9 @@
       <c r="G2" t="n">
         <v>0.913923733715832</v>
       </c>
-      <c r="H2"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -520,7 +522,9 @@
       <c r="G3" t="n">
         <v>0.0515375128493991</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -544,7 +548,9 @@
       <c r="G4" t="n">
         <v>0.416390784715524</v>
       </c>
-      <c r="H4"/>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -568,7 +574,9 @@
       <c r="G5" t="n">
         <v>0.861173722353446</v>
       </c>
-      <c r="H5"/>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -592,7 +600,9 @@
       <c r="G6" t="n">
         <v>0.0018064637219179</v>
       </c>
-      <c r="H6"/>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -616,7 +626,9 @@
       <c r="G7" t="n">
         <v>0.114651371099957</v>
       </c>
-      <c r="H7"/>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -640,7 +652,9 @@
       <c r="G8" t="n">
         <v>0.752538905554521</v>
       </c>
-      <c r="H8"/>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -664,7 +678,9 @@
       <c r="G9" t="n">
         <v>0.498163118898279</v>
       </c>
-      <c r="H9"/>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -688,7 +704,9 @@
       <c r="G10" t="n">
         <v>0.686398262725029</v>
       </c>
-      <c r="H10"/>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -712,7 +730,9 @@
       <c r="G11" t="n">
         <v>0.795450291474774</v>
       </c>
-      <c r="H11"/>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -736,7 +756,9 @@
       <c r="G12" t="n">
         <v>0.870356268103246</v>
       </c>
-      <c r="H12"/>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -760,7 +782,9 @@
       <c r="G13" t="n">
         <v>0.152244682063856</v>
       </c>
-      <c r="H13"/>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -810,7 +834,9 @@
       <c r="G15" t="n">
         <v>0.104669076341271</v>
       </c>
-      <c r="H15"/>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -834,7 +860,9 @@
       <c r="G16" t="n">
         <v>0.101488572392428</v>
       </c>
-      <c r="H16"/>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -858,7 +886,9 @@
       <c r="G17" t="n">
         <v>0.468730860724079</v>
       </c>
-      <c r="H17"/>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -882,7 +912,9 @@
       <c r="G18" t="n">
         <v>0.0306395409429453</v>
       </c>
-      <c r="H18"/>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -906,7 +938,9 @@
       <c r="G19" t="n">
         <v>0.0145049136480768</v>
       </c>
-      <c r="H19"/>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -930,7 +964,9 @@
       <c r="G20" t="n">
         <v>0.247133573198254</v>
       </c>
-      <c r="H20"/>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -954,7 +990,9 @@
       <c r="G21" t="n">
         <v>0.576921530981013</v>
       </c>
-      <c r="H21"/>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -978,7 +1016,9 @@
       <c r="G22" t="n">
         <v>0.143041609451352</v>
       </c>
-      <c r="H22"/>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1002,7 +1042,9 @@
       <c r="G23" t="n">
         <v>0.370302386119609</v>
       </c>
-      <c r="H23"/>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1026,7 +1068,9 @@
       <c r="G24" t="n">
         <v>0.130626389933383</v>
       </c>
-      <c r="H24"/>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1050,7 +1094,9 @@
       <c r="G25" t="n">
         <v>0.157122997107345</v>
       </c>
-      <c r="H25"/>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1074,7 +1120,9 @@
       <c r="G26" t="n">
         <v>0.000207431366230397</v>
       </c>
-      <c r="H26"/>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1098,7 +1146,9 @@
       <c r="G27" t="n">
         <v>0.283974650684971</v>
       </c>
-      <c r="H27"/>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">

</xml_diff>